<commit_message>
Finished claims-header and claims-details
And renamed some files too
</commit_message>
<xml_diff>
--- a/greenplum/datawarehouse/QA/qa-all-db-checks/medicaid/outputs/dw-claims-counting.xlsx
+++ b/greenplum/datawarehouse/QA/qa-all-db-checks/medicaid/outputs/dw-claims-counting.xlsx
@@ -1,227 +1,220 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\XIAORUI\dw\outputs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F9CD88-A9A3-4449-A3FE-902BCA37E21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="1575" windowWidth="17760" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Count of distinct claims" sheetId="1" r:id="rId1"/>
+    <sheet name="Count of distinct claims" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="65">
-  <si>
-    <t>Count of distinct claims across SPC and TACC servers</t>
-  </si>
-  <si>
-    <t>Run time: 2022-11-02 16:23:24</t>
-  </si>
-  <si>
-    <t>year_fy</t>
-  </si>
-  <si>
-    <t>TACmcd_HEAD</t>
-  </si>
-  <si>
-    <t>TACmcd_DET</t>
-  </si>
-  <si>
-    <t>DW_HEAD</t>
-  </si>
-  <si>
-    <t>DW_DET</t>
-  </si>
-  <si>
-    <t>SPC_HEAD</t>
-  </si>
-  <si>
-    <t>SPC_DET</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>45636958</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>88630037</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>87542296</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>91770349</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>96259441</t>
-  </si>
-  <si>
-    <t>96259566</t>
-  </si>
-  <si>
-    <t>96259442</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>103704132</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>108809719</t>
-  </si>
-  <si>
-    <t>109481883</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>109194207</t>
-  </si>
-  <si>
-    <t>109194320</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>106324148</t>
-  </si>
-  <si>
-    <t>106324149</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>111404359</t>
-  </si>
-  <si>
-    <t>HTW</t>
-  </si>
-  <si>
-    <t>672173</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>949947819</t>
-  </si>
-  <si>
-    <t>949947944</t>
-  </si>
-  <si>
-    <t>949947810</t>
-  </si>
-  <si>
-    <t>Difference between counts (Raw data count - DW count)</t>
-  </si>
-  <si>
-    <t>DW_V_TACm_HEAD</t>
-  </si>
-  <si>
-    <t>DW_V_TACm_DET</t>
-  </si>
-  <si>
-    <t>spacer1</t>
-  </si>
-  <si>
-    <t>spacer2</t>
-  </si>
-  <si>
-    <t>DW_V_SPC_HEAD</t>
-  </si>
-  <si>
-    <t>DW_V_SPC_DET</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>-672164</t>
-  </si>
-  <si>
-    <t>-113</t>
-  </si>
-  <si>
-    <t>-1</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>-949947810</t>
-  </si>
-  <si>
-    <t>Column Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Fiscal Year</t>
-  </si>
-  <si>
-    <t>Count of distinct claims in TACC medicaid schema - headers</t>
-  </si>
-  <si>
-    <t>Count of distinct claims in TACC medicaid schema - details</t>
-  </si>
-  <si>
-    <t>Count of distinct claims in dw_staging.claim_header</t>
-  </si>
-  <si>
-    <t>Count of distinct claims in dw_staging.claim_detail</t>
-  </si>
-  <si>
-    <t>Count of distinct claims in SPC medicaid schema headers joined to procs</t>
-  </si>
-  <si>
-    <t>Count of distinct claims in SPC medicaid schema details joined to procs</t>
-  </si>
-  <si>
-    <t/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+  <si>
+    <t xml:space="preserve">Count of distinct claims across SPC and TACC servers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run time: 2022-11-15 13:20:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_fy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TACmcd_HEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TACmcd_DET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DW_HEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DW_DET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPC_HEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPC_DET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45636958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88630037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87542296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91770349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96259441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96259566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96259442</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">103704132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">108809719</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109481883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109194207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109194320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">106324148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">106324149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111404359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">672173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">949947819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">949947944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">949947810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference between counts (Raw data count - DW count)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DW_V_TACm_HEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DW_V_TACm_DET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spacer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spacer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DW_V_SPC_HEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DW_V_SPC_DET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-672164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-949947810</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Column Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of distinct claims in TACC medicaid schema - headers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of distinct claims in TACC medicaid schema - details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of distinct claims in dw_staging.claim_header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of distinct claims in dw_staging.claim_detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of distinct claims in SPC medicaid schema headers joined to procs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of distinct claims in SPC medicaid schema details joined to procs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -257,15 +250,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -547,32 +531,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="15.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="13.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="9.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="9.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="13.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="12.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="9.15" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -595,7 +581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -611,14 +597,14 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>45636958</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>45636958</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -634,14 +620,14 @@
       <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>88630037</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>88630037</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -657,14 +643,14 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>87542296</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="n">
         <v>87542296</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -680,14 +666,14 @@
       <c r="E8" t="s">
         <v>16</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>91770349</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="n">
         <v>91770349</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -703,14 +689,14 @@
       <c r="E9" t="s">
         <v>20</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>96259441</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>96259566</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -726,14 +712,14 @@
       <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="n">
         <v>103704132</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="n">
         <v>103704132</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -749,14 +735,14 @@
       <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="n">
         <v>108809719</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="n">
         <v>108809719</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -772,14 +758,14 @@
       <c r="E12" t="s">
         <v>28</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="n">
         <v>109194207</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="n">
         <v>109194207</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -795,14 +781,14 @@
       <c r="E13" t="s">
         <v>31</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="n">
         <v>106324148</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="n">
         <v>106324148</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -818,14 +804,14 @@
       <c r="E14" t="s">
         <v>33</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="n">
         <v>111404359</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="n">
         <v>111404359</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -841,14 +827,14 @@
       <c r="E15" t="s">
         <v>36</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="n">
         <v>672173</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="n">
         <v>672173</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -864,19 +850,19 @@
       <c r="E16" t="s">
         <v>40</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="n">
         <v>0</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -887,10 +873,10 @@
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
         <v>46</v>
@@ -899,7 +885,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -909,6 +895,8 @@
       <c r="C20" t="s">
         <v>36</v>
       </c>
+      <c r="D20"/>
+      <c r="E20"/>
       <c r="F20" t="s">
         <v>36</v>
       </c>
@@ -916,7 +904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -926,6 +914,8 @@
       <c r="C21" t="s">
         <v>36</v>
       </c>
+      <c r="D21"/>
+      <c r="E21"/>
       <c r="F21" t="s">
         <v>36</v>
       </c>
@@ -933,7 +923,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -943,6 +933,8 @@
       <c r="C22" t="s">
         <v>36</v>
       </c>
+      <c r="D22"/>
+      <c r="E22"/>
       <c r="F22" t="s">
         <v>36</v>
       </c>
@@ -950,7 +942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -960,6 +952,8 @@
       <c r="C23" t="s">
         <v>36</v>
       </c>
+      <c r="D23"/>
+      <c r="E23"/>
       <c r="F23" t="s">
         <v>36</v>
       </c>
@@ -967,7 +961,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -977,6 +971,8 @@
       <c r="C24" t="s">
         <v>48</v>
       </c>
+      <c r="D24"/>
+      <c r="E24"/>
       <c r="F24" t="s">
         <v>36</v>
       </c>
@@ -984,7 +980,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -994,6 +990,8 @@
       <c r="C25" t="s">
         <v>36</v>
       </c>
+      <c r="D25"/>
+      <c r="E25"/>
       <c r="F25" t="s">
         <v>36</v>
       </c>
@@ -1001,7 +999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1011,6 +1009,8 @@
       <c r="C26" t="s">
         <v>49</v>
       </c>
+      <c r="D26"/>
+      <c r="E26"/>
       <c r="F26" t="s">
         <v>49</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1028,6 +1028,8 @@
       <c r="C27" t="s">
         <v>50</v>
       </c>
+      <c r="D27"/>
+      <c r="E27"/>
       <c r="F27" t="s">
         <v>36</v>
       </c>
@@ -1035,7 +1037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1045,6 +1047,8 @@
       <c r="C28" t="s">
         <v>51</v>
       </c>
+      <c r="D28"/>
+      <c r="E28"/>
       <c r="F28" t="s">
         <v>36</v>
       </c>
@@ -1052,7 +1056,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1062,6 +1066,8 @@
       <c r="C29" t="s">
         <v>36</v>
       </c>
+      <c r="D29"/>
+      <c r="E29"/>
       <c r="F29" t="s">
         <v>36</v>
       </c>
@@ -1069,7 +1075,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1079,6 +1085,8 @@
       <c r="C30" t="s">
         <v>35</v>
       </c>
+      <c r="D30"/>
+      <c r="E30"/>
       <c r="F30" t="s">
         <v>35</v>
       </c>
@@ -1086,7 +1094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1096,6 +1104,8 @@
       <c r="C31" t="s">
         <v>53</v>
       </c>
+      <c r="D31"/>
+      <c r="E31"/>
       <c r="F31" t="s">
         <v>54</v>
       </c>
@@ -1103,78 +1113,72 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" t="s">
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35" t="s">
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37" t="s">
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" t="s">
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" t="s">
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40" t="s">
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>